<commit_message>
Add validation for create test and import question
</commit_message>
<xml_diff>
--- a/Uploads/ImportQuestionTemplate.xlsx
+++ b/Uploads/ImportQuestionTemplate.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t>Type</t>
   </si>
@@ -87,18 +87,6 @@
     <t>Content</t>
   </si>
   <si>
-    <t>Answser 1</t>
-  </si>
-  <si>
-    <t>Answser 2</t>
-  </si>
-  <si>
-    <t>Answser 3</t>
-  </si>
-  <si>
-    <t>Answser 4</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -208,6 +196,39 @@
   </si>
   <si>
     <t>table1.png,table2.png</t>
+  </si>
+  <si>
+    <t>Answer 1</t>
+  </si>
+  <si>
+    <t>Answer 3</t>
+  </si>
+  <si>
+    <t>Answer 2</t>
+  </si>
+  <si>
+    <t>Answer 4</t>
+  </si>
+  <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>fsfsdfsdfsd sdfsdf</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>dsfsd</t>
+  </si>
+  <si>
+    <t>sdfs</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>sdfds</t>
   </si>
 </sst>
 </file>
@@ -627,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,7 +674,7 @@
     <row r="1" spans="2:15" ht="11.25" customHeight="1"/>
     <row r="2" spans="2:15" ht="13.5" customHeight="1">
       <c r="B2" s="10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -688,46 +709,46 @@
     <row r="4" spans="2:15" ht="12.75" customHeight="1"/>
     <row r="5" spans="2:15" s="9" customFormat="1" ht="25.5" customHeight="1">
       <c r="B5" s="7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="M5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -735,39 +756,39 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J6" s="6">
         <v>2</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:15">
@@ -775,39 +796,39 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J7" s="6">
         <v>2</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -815,38 +836,38 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="O8" s="1"/>
     </row>
@@ -855,28 +876,36 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
@@ -885,28 +914,36 @@
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="J10" s="6">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
@@ -915,23 +952,35 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="2:15">
@@ -939,23 +988,35 @@
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="2:15">
@@ -1104,7 +1165,7 @@
     </row>
     <row r="22" spans="2:15">
       <c r="B22" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>

</xml_diff>